<commit_message>
Prise en compte des modifications lors de la conference video
</commit_message>
<xml_diff>
--- a/documents/workbook.xlsx
+++ b/documents/workbook.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Feuille de présence</t>
   </si>
@@ -88,25 +88,10 @@
     <t xml:space="preserve">Place :   </t>
   </si>
   <si>
-    <t>Formation : une formation</t>
+    <t>Formation : qh bon</t>
   </si>
   <si>
-    <t>Renault Trucks</t>
-  </si>
-  <si>
-    <t>BADINI Adama</t>
-  </si>
-  <si>
-    <t>ABDOULKARIM ALI</t>
-  </si>
-  <si>
-    <t>ADAMNE Bertin</t>
-  </si>
-  <si>
-    <t>CHEFOU IDI</t>
-  </si>
-  <si>
-    <t>Armel Kadje</t>
+    <t>moi ahbo</t>
   </si>
 </sst>
 </file>
@@ -1750,9 +1735,7 @@
       <c r="F3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="G3" s="7"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -1862,7 +1845,7 @@
     </row>
     <row customHeight="1" ht="27.75" r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
@@ -1879,9 +1862,7 @@
       <c r="O8" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>20</v>
-      </c>
+      <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>
       <c r="D9" s="23"/>
@@ -1897,9 +1878,7 @@
       <c r="O9" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>21</v>
-      </c>
+      <c r="A10" s="24"/>
       <c r="B10" s="21"/>
       <c r="C10" s="22"/>
       <c r="D10" s="23"/>
@@ -1915,9 +1894,7 @@
       <c r="O10" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>19</v>
-      </c>
+      <c r="A11" s="25"/>
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
       <c r="D11" s="23"/>
@@ -1933,9 +1910,7 @@
       <c r="O11" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>22</v>
-      </c>
+      <c r="A12" s="25"/>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
       <c r="D12" s="23"/>
@@ -1951,9 +1926,7 @@
       <c r="O12" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="24"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
       <c r="D13" s="23"/>
@@ -1969,9 +1942,7 @@
       <c r="O13" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>23</v>
-      </c>
+      <c r="A14" s="26"/>
       <c r="B14" s="23"/>
       <c r="C14" s="22"/>
       <c r="D14" s="23"/>
@@ -1987,9 +1958,7 @@
       <c r="O14" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="A15" s="25"/>
       <c r="B15" s="23"/>
       <c r="C15" s="22"/>
       <c r="D15" s="23"/>
@@ -2005,9 +1974,7 @@
       <c r="O15" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>23</v>
-      </c>
+      <c r="A16" s="27"/>
       <c r="B16" s="23"/>
       <c r="C16" s="22"/>
       <c r="D16" s="23"/>
@@ -2023,9 +1990,7 @@
       <c r="O16" s="21"/>
     </row>
     <row customHeight="1" ht="27.75" r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>22</v>
-      </c>
+      <c r="A17" s="27"/>
       <c r="B17" s="23"/>
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
@@ -2041,9 +2006,7 @@
       <c r="O17" s="21"/>
     </row>
     <row customHeight="1" ht="24" r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>23</v>
-      </c>
+      <c r="A18" s="27"/>
       <c r="B18" s="23"/>
       <c r="C18" s="22"/>
       <c r="D18" s="23"/>

</xml_diff>